<commit_message>
1. added CFG representation (CFGBuilder.CFG < LinkedList) 2. changed CommandBlocks: 	- if t1 != null, command is an assignment into t1 (t1 = something) 	- if t2 != null, command uses t2 (somthing = ...t2...) 	- if t3 != null, command uses t3 (somthing = ...t3...)
</commit_message>
<xml_diff>
--- a/ex4_command_list.xlsx
+++ b/ex4_command_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\COMPILATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1FE57A-E324-42CE-BAA5-82395FE87F54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897E354-8740-47AB-842E-35BB4B50F626}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1B6E2A60-7A13-41B5-B39D-809F7A69E663}"/>
+    <workbookView xWindow="38280" yWindow="-3960" windowWidth="18240" windowHeight="28440" xr2:uid="{1B6E2A60-7A13-41B5-B39D-809F7A69E663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>PrintInt</t>
   </si>
   <si>
-    <t>printed temp</t>
-  </si>
-  <si>
     <t>PrintString</t>
   </si>
   <si>
@@ -75,24 +72,12 @@
     <t>lw</t>
   </si>
   <si>
-    <t>t1 = offset(t2)</t>
-  </si>
-  <si>
-    <t>ButtomElement</t>
-  </si>
-  <si>
     <t>start analysis from this block</t>
   </si>
   <si>
     <t>sw</t>
   </si>
   <si>
-    <t>t1 = $reg (v0\fp..)</t>
-  </si>
-  <si>
-    <t>$t1 = t2</t>
-  </si>
-  <si>
     <t>$reg = t2</t>
   </si>
   <si>
@@ -105,27 +90,15 @@
     <t>lb</t>
   </si>
   <si>
-    <t>t1 = const</t>
-  </si>
-  <si>
     <t>sll</t>
   </si>
   <si>
     <t>t1 = sll by offset (t2)</t>
   </si>
   <si>
-    <t>some const place = t1</t>
-  </si>
-  <si>
-    <t>t2[offset] = t1</t>
-  </si>
-  <si>
     <t>sb</t>
   </si>
   <si>
-    <t>t2[offset] = const</t>
-  </si>
-  <si>
     <t>li</t>
   </si>
   <si>
@@ -177,58 +150,85 @@
     <t>jr</t>
   </si>
   <si>
-    <t>return (jr $ra)</t>
-  </si>
-  <si>
     <t>jalr</t>
   </si>
   <si>
-    <t>jump to t1 and link</t>
-  </si>
-  <si>
     <t>blt</t>
   </si>
   <si>
-    <t>if (t1 &lt; t2) jump to label</t>
-  </si>
-  <si>
-    <t>if (t1 &lt; $zero) jump to label</t>
-  </si>
-  <si>
     <t>bltz</t>
   </si>
   <si>
-    <t>if (t1 &gt; t2) jump to label</t>
-  </si>
-  <si>
     <t>bge</t>
   </si>
   <si>
-    <t>if (t1 != t2) jump to label</t>
-  </si>
-  <si>
     <t>bne</t>
   </si>
   <si>
     <t>bnez</t>
   </si>
   <si>
-    <t>if (t1 != $zero) jump to label</t>
-  </si>
-  <si>
     <t>beq</t>
   </si>
   <si>
     <t>beqz</t>
   </si>
   <si>
-    <t>if (t1 == t2) jump to label</t>
-  </si>
-  <si>
-    <t>if (t1 == $zero) jump to label</t>
-  </si>
-  <si>
     <t>printed string's address temp</t>
+  </si>
+  <si>
+    <t>t1 = t2</t>
+  </si>
+  <si>
+    <t>t1 = mem[t2+offset]</t>
+  </si>
+  <si>
+    <t>t1 = mem[some place]</t>
+  </si>
+  <si>
+    <t>t1 = $reg (v0\a0\fp..)</t>
+  </si>
+  <si>
+    <t>mem[some place] = t2</t>
+  </si>
+  <si>
+    <t>mem[t3+offset] = t2</t>
+  </si>
+  <si>
+    <t>mem[t3+offset]= const</t>
+  </si>
+  <si>
+    <t>printed int</t>
+  </si>
+  <si>
+    <t>return (eg. jr $ra)</t>
+  </si>
+  <si>
+    <t>jump to address t2 and link</t>
+  </si>
+  <si>
+    <t>if (t2 != $zero) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 != t3) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 == $zero) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 == t3) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 &gt; t3) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 &lt; $zero) jump to label</t>
+  </si>
+  <si>
+    <t>if (t2 &lt; t3) jump to label</t>
+  </si>
+  <si>
+    <t>buttomElement</t>
   </si>
 </sst>
 </file>
@@ -341,7 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
@@ -353,6 +353,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,7 +678,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,47 +686,47 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -771,11 +772,11 @@
         <v>8</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
@@ -786,14 +787,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -804,10 +805,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
@@ -824,10 +825,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -844,10 +845,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -864,10 +865,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -884,10 +885,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -904,10 +905,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -924,16 +925,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>7</v>
@@ -944,19 +945,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
+        <v>53</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
@@ -964,19 +965,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>7</v>
+      <c r="E16" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>7</v>
@@ -984,19 +985,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>7</v>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>7</v>
@@ -1004,10 +1005,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
@@ -1024,10 +1025,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -1044,10 +1045,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>2</v>
@@ -1064,10 +1065,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>2</v>
@@ -1084,10 +1085,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
@@ -1104,10 +1105,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>2</v>
@@ -1124,10 +1125,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>2</v>
@@ -1144,10 +1145,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>2</v>
@@ -1164,10 +1165,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>2</v>
@@ -1192,10 +1193,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
@@ -1212,10 +1213,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
@@ -1232,16 +1233,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
+        <v>57</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>7</v>
@@ -1252,19 +1253,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>2</v>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>7</v>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>5</v>
@@ -1272,16 +1273,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>7</v>
@@ -1292,19 +1293,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>2</v>
+        <v>59</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>7</v>
+      <c r="E33" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>5</v>
@@ -1312,16 +1313,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>7</v>
@@ -1332,19 +1333,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>7</v>
+      <c r="E35" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>5</v>
@@ -1352,19 +1353,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>7</v>
+      <c r="E36" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>5</v>
@@ -1372,16 +1373,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>7</v>
@@ -1403,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
out of bounds fix
</commit_message>
<xml_diff>
--- a/ex4_command_list.xlsx
+++ b/ex4_command_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\COMPILATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025851BA-7382-42BB-9298-FCBF49F5E723}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DB81BC-322D-4FCE-B623-8B34D4397ACD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1B6E2A60-7A13-41B5-B39D-809F7A69E663}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
   <si>
     <t>commandName</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>buttomElement</t>
+  </si>
+  <si>
+    <t>bgt</t>
+  </si>
+  <si>
+    <t>if (t2 &gt;= t3) jump to label</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22451AC9-6FFD-41CC-AB6F-BCA4432F9A57}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1339,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>62</v>
@@ -1353,10 +1359,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>7</v>
@@ -1373,10 +1379,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>7</v>
@@ -1384,38 +1390,58 @@
       <c r="D37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>7</v>
+      <c r="E37" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>